<commit_message>
Fix some bugs and apply data type for number values.
</commit_message>
<xml_diff>
--- a/management/src/main/resources/DepartmentMeetings_template.xlsx
+++ b/management/src/main/resources/DepartmentMeetings_template.xlsx
@@ -72,7 +72,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="24" uniqueCount="24">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="22" uniqueCount="22">
   <si>
     <t>${record.region}</t>
   </si>
@@ -120,12 +120,6 @@
   </si>
   <si>
     <t>${record.purpose}</t>
-  </si>
-  <si>
-    <t>会议主题</t>
-  </si>
-  <si>
-    <t>${record.subject}</t>
   </si>
   <si>
     <t>费用预算</t>
@@ -519,18 +513,18 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:L4"/>
+  <dimension ref="A1:K4"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="M4" sqref="M4"/>
+      <selection activeCell="I1" sqref="I1:I1048576"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="12" width="18.5703125" customWidth="1"/>
+    <col min="1" max="11" width="18.5703125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:12" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:11" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A1" s="2" t="s">
         <v>9</v>
       </c>
@@ -564,11 +558,8 @@
       <c r="K1" s="2" t="s">
         <v>20</v>
       </c>
-      <c r="L1" s="2" t="s">
-        <v>22</v>
-      </c>
     </row>
-    <row r="2" spans="1:12" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:11" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A2" s="3" t="s">
         <v>4</v>
       </c>
@@ -602,25 +593,20 @@
       <c r="K2" t="s">
         <v>21</v>
       </c>
-      <c r="L2" t="s">
-        <v>23</v>
-      </c>
     </row>
-    <row r="3" spans="1:12" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:11" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="G3" s="1"/>
       <c r="H3" s="1"/>
       <c r="I3" s="1"/>
       <c r="J3" s="1"/>
       <c r="K3" s="1"/>
-      <c r="L3" s="1"/>
     </row>
-    <row r="4" spans="1:12" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:11" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="G4" s="1"/>
       <c r="H4" s="1"/>
       <c r="I4" s="1"/>
       <c r="J4" s="1"/>
       <c r="K4" s="1"/>
-      <c r="L4" s="1"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>

<commit_message>
1. Add more column for lost/new customer. 2. Export support for lost/new customer. 3. Export number of people for department meeting.
</commit_message>
<xml_diff>
--- a/management/src/main/resources/DepartmentMeetings_template.xlsx
+++ b/management/src/main/resources/DepartmentMeetings_template.xlsx
@@ -1,7 +1,7 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="14420"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="16925"/>
   <workbookPr filterPrivacy="1" defaultThemeVersion="124226"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="0" windowWidth="15990" windowHeight="3915"/>
@@ -10,7 +10,6 @@
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
   </sheets>
   <calcPr calcId="0"/>
-  <oleSize ref="A1"/>
 </workbook>
 </file>
 
@@ -73,7 +72,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="22" uniqueCount="22">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="24" uniqueCount="24">
   <si>
     <t>${record.region}</t>
   </si>
@@ -139,12 +138,18 @@
   </si>
   <si>
     <t>${record.salesPersonFullName}</t>
+  </si>
+  <si>
+    <t>参会人数</t>
+  </si>
+  <si>
+    <t>${record.numberOfPeople}</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
   <numFmts count="1">
     <numFmt numFmtId="164" formatCode="yyyy\-mm\-dd;@"/>
   </numFmts>
@@ -303,6 +308,23 @@
         <a:font script="Viet" typeface="Times New Roman"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
         <a:font script="Geor" typeface="Sylfaen"/>
+        <a:font script="Armn" typeface="Arial"/>
+        <a:font script="Bugi" typeface="Leelawadee UI"/>
+        <a:font script="Bopo" typeface="Microsoft JhengHei"/>
+        <a:font script="Java" typeface="Javanese Text"/>
+        <a:font script="Lisu" typeface="Segoe UI"/>
+        <a:font script="Mymr" typeface="Myanmar Text"/>
+        <a:font script="Nkoo" typeface="Ebrima"/>
+        <a:font script="Olck" typeface="Nirmala UI"/>
+        <a:font script="Osma" typeface="Ebrima"/>
+        <a:font script="Phag" typeface="Phagspa"/>
+        <a:font script="Syrn" typeface="Estrangelo Edessa"/>
+        <a:font script="Syrj" typeface="Estrangelo Edessa"/>
+        <a:font script="Syre" typeface="Estrangelo Edessa"/>
+        <a:font script="Sora" typeface="Nirmala UI"/>
+        <a:font script="Tale" typeface="Microsoft Tai Le"/>
+        <a:font script="Talu" typeface="Microsoft New Tai Lue"/>
+        <a:font script="Tfng" typeface="Ebrima"/>
       </a:majorFont>
       <a:minorFont>
         <a:latin typeface="Calibri" panose="020F0502020204030204"/>
@@ -338,6 +360,23 @@
         <a:font script="Viet" typeface="Arial"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
         <a:font script="Geor" typeface="Sylfaen"/>
+        <a:font script="Armn" typeface="Arial"/>
+        <a:font script="Bugi" typeface="Leelawadee UI"/>
+        <a:font script="Bopo" typeface="Microsoft JhengHei"/>
+        <a:font script="Java" typeface="Javanese Text"/>
+        <a:font script="Lisu" typeface="Segoe UI"/>
+        <a:font script="Mymr" typeface="Myanmar Text"/>
+        <a:font script="Nkoo" typeface="Ebrima"/>
+        <a:font script="Olck" typeface="Nirmala UI"/>
+        <a:font script="Osma" typeface="Ebrima"/>
+        <a:font script="Phag" typeface="Phagspa"/>
+        <a:font script="Syrn" typeface="Estrangelo Edessa"/>
+        <a:font script="Syrj" typeface="Estrangelo Edessa"/>
+        <a:font script="Syre" typeface="Estrangelo Edessa"/>
+        <a:font script="Sora" typeface="Nirmala UI"/>
+        <a:font script="Tale" typeface="Microsoft Tai Le"/>
+        <a:font script="Talu" typeface="Microsoft New Tai Lue"/>
+        <a:font script="Tfng" typeface="Ebrima"/>
       </a:minorFont>
     </a:fontScheme>
     <a:fmtScheme name="Office">
@@ -514,18 +553,19 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:K4"/>
+  <dimension ref="A1:L4"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D3" sqref="D3"/>
+      <selection activeCell="F12" sqref="F12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="11" width="18.5703125" customWidth="1"/>
+    <col min="12" max="12" width="9.85546875" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:11" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:12" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A1" s="2" t="s">
         <v>8</v>
       </c>
@@ -559,8 +599,11 @@
       <c r="K1" s="2" t="s">
         <v>19</v>
       </c>
+      <c r="L1" s="2" t="s">
+        <v>22</v>
+      </c>
     </row>
-    <row r="2" spans="1:11" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:12" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A2" s="3" t="s">
         <v>3</v>
       </c>
@@ -594,15 +637,18 @@
       <c r="K2" t="s">
         <v>20</v>
       </c>
+      <c r="L2" t="s">
+        <v>23</v>
+      </c>
     </row>
-    <row r="3" spans="1:11" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:12" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="G3" s="1"/>
       <c r="H3" s="1"/>
       <c r="I3" s="1"/>
       <c r="J3" s="1"/>
       <c r="K3" s="1"/>
     </row>
-    <row r="4" spans="1:11" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:12" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="G4" s="1"/>
       <c r="H4" s="1"/>
       <c r="I4" s="1"/>

</xml_diff>

<commit_message>
1. Enable data export for all roles. 2. Add planDate for department meetings
</commit_message>
<xml_diff>
--- a/management/src/main/resources/DepartmentMeetings_template.xlsx
+++ b/management/src/main/resources/DepartmentMeetings_template.xlsx
@@ -1,7 +1,7 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="16925"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="17726"/>
   <workbookPr filterPrivacy="1" defaultThemeVersion="124226"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="0" windowWidth="15990" windowHeight="3915"/>
@@ -39,7 +39,7 @@
             <family val="2"/>
           </rPr>
           <t xml:space="preserve">
-jx:area(lastCell="L2")</t>
+jx:area(lastCell="M2")</t>
         </r>
       </text>
     </comment>
@@ -63,7 +63,7 @@
             <family val="2"/>
           </rPr>
           <t xml:space="preserve">
-jx:each(items="data" var="record" lastCell="L2")</t>
+jx:each(items="data" var="record" lastCell="M2")</t>
         </r>
       </text>
     </comment>
@@ -72,7 +72,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="24" uniqueCount="24">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="26" uniqueCount="26">
   <si>
     <t>${record.region}</t>
   </si>
@@ -144,6 +144,12 @@
   </si>
   <si>
     <t>${record.numberOfPeople}</t>
+  </si>
+  <si>
+    <t>拟召开日期</t>
+  </si>
+  <si>
+    <t>${record.planDate}</t>
   </si>
 </sst>
 </file>
@@ -553,19 +559,20 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:L4"/>
+  <dimension ref="A1:M4"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="F12" sqref="F12"/>
+      <selection activeCell="M2" sqref="M2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="11" width="18.5703125" customWidth="1"/>
     <col min="12" max="12" width="9.85546875" customWidth="1"/>
+    <col min="13" max="13" width="18.42578125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:12" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:13" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A1" s="2" t="s">
         <v>8</v>
       </c>
@@ -602,8 +609,11 @@
       <c r="L1" s="2" t="s">
         <v>22</v>
       </c>
+      <c r="M1" s="2" t="s">
+        <v>24</v>
+      </c>
     </row>
-    <row r="2" spans="1:12" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:13" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A2" s="3" t="s">
         <v>3</v>
       </c>
@@ -640,15 +650,18 @@
       <c r="L2" t="s">
         <v>23</v>
       </c>
+      <c r="M2" s="3" t="s">
+        <v>25</v>
+      </c>
     </row>
-    <row r="3" spans="1:12" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:13" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="G3" s="1"/>
       <c r="H3" s="1"/>
       <c r="I3" s="1"/>
       <c r="J3" s="1"/>
       <c r="K3" s="1"/>
     </row>
-    <row r="4" spans="1:12" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:13" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="G4" s="1"/>
       <c r="H4" s="1"/>
       <c r="I4" s="1"/>

</xml_diff>